<commit_message>
All data for v2
</commit_message>
<xml_diff>
--- a/model/data/All_EVProject2013Qtly_Residential_Hr.xlsx
+++ b/model/data/All_EVProject2013Qtly_Residential_Hr.xlsx
@@ -72,7 +72,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="173" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -115,7 +115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -431,7 +431,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomRight" activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1666,6 +1666,18 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="L2:L25">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>